<commit_message>
OPtion to add stocks and chose between different stocks
</commit_message>
<xml_diff>
--- a/backtest_results.xlsx
+++ b/backtest_results.xlsx
@@ -476,278 +476,278 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45566.73307043832</v>
+        <v>45566.82485457524</v>
       </c>
       <c r="B2" t="n">
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="C2" t="n">
-        <v>5708.75</v>
+        <v>48.51067352294922</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7006787825706153</v>
+        <v>20.61402011924086</v>
       </c>
       <c r="E2" t="n">
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="F2" t="n">
-        <v>4655.099764615722</v>
+        <v>1983.274856799464</v>
       </c>
       <c r="G2" t="n">
-        <v>655.0997646157221</v>
+        <v>983.274856799464</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45597.73307043832</v>
+        <v>45597.82485457524</v>
       </c>
       <c r="B3" t="n">
         <v>1000</v>
       </c>
       <c r="C3" t="n">
-        <v>5728.7998046875</v>
+        <v>49.56356048583984</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1745566321207045</v>
+        <v>20.17611305962768</v>
       </c>
       <c r="E3" t="n">
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="F3" t="n">
-        <v>5814.80169552914</v>
+        <v>3924.41867579446</v>
       </c>
       <c r="G3" t="n">
-        <v>814.8016955291396</v>
+        <v>1924.41867579446</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45627.73307043832</v>
+        <v>45627.82485457524</v>
       </c>
       <c r="B4" t="n">
         <v>1000</v>
       </c>
       <c r="C4" t="n">
-        <v>6032.3798828125</v>
+        <v>46.4828987121582</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1657720533896095</v>
+        <v>21.51328827817782</v>
       </c>
       <c r="E4" t="n">
-        <v>6000</v>
+        <v>3000</v>
       </c>
       <c r="F4" t="n">
-        <v>6916.141519011042</v>
+        <v>5994.212121341945</v>
       </c>
       <c r="G4" t="n">
-        <v>916.141519011042</v>
+        <v>2994.212121341945</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45658.73307043832</v>
+        <v>45658.82485457524</v>
       </c>
       <c r="B5" t="n">
         <v>1000</v>
       </c>
       <c r="C5" t="n">
-        <v>5881.6298828125</v>
+        <v>42.75</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1700208989556167</v>
+        <v>23.39181286549708</v>
       </c>
       <c r="E5" t="n">
-        <v>7000</v>
+        <v>4000</v>
       </c>
       <c r="F5" t="n">
-        <v>8045.709398609679</v>
+        <v>8244.738415715574</v>
       </c>
       <c r="G5" t="n">
-        <v>1045.709398609679</v>
+        <v>4244.738415715574</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45689.73307043832</v>
+        <v>45689.82485457524</v>
       </c>
       <c r="B6" t="n">
-        <v>1000</v>
+        <v>6338</v>
       </c>
       <c r="C6" t="n">
-        <v>6040.52978515625</v>
+        <v>48.36999893188477</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1655483931984507</v>
+        <v>131.0316340698136</v>
       </c>
       <c r="E6" t="n">
-        <v>8000</v>
+        <v>10338</v>
       </c>
       <c r="F6" t="n">
-        <v>9145.563290835897</v>
+        <v>20851.2918096093</v>
       </c>
       <c r="G6" t="n">
-        <v>1145.563290835897</v>
+        <v>10513.2918096093</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45717.73307043832</v>
+        <v>45717.82485457524</v>
       </c>
       <c r="B7" t="n">
         <v>1000</v>
       </c>
       <c r="C7" t="n">
-        <v>5954.5</v>
+        <v>48.65999984741211</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1679402132840709</v>
+        <v>20.55076044257701</v>
       </c>
       <c r="E7" t="n">
-        <v>9000</v>
+        <v>11338</v>
       </c>
       <c r="F7" t="n">
-        <v>10261.3077186321</v>
+        <v>22828.48045297485</v>
       </c>
       <c r="G7" t="n">
-        <v>1261.307718632101</v>
+        <v>11490.48045297485</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45748.73307043832</v>
+        <v>45748.82485457524</v>
       </c>
       <c r="B8" t="n">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="C8" t="n">
-        <v>5633.06982421875</v>
+        <v>56.90999984741211</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5325692905672565</v>
+        <v>17.57160433458468</v>
       </c>
       <c r="E8" t="n">
-        <v>12000</v>
+        <v>12338</v>
       </c>
       <c r="F8" t="n">
-        <v>13799.53841839122</v>
+        <v>24519.04448991796</v>
       </c>
       <c r="G8" t="n">
-        <v>1799.538418391221</v>
+        <v>12181.04448991796</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45778.73307043832</v>
+        <v>45778.82485457524</v>
       </c>
       <c r="B9" t="n">
         <v>1000</v>
       </c>
       <c r="C9" t="n">
-        <v>5604.14013671875</v>
+        <v>58.72999954223633</v>
       </c>
       <c r="D9" t="n">
-        <v>0.1784395064370222</v>
+        <v>17.02707317885877</v>
       </c>
       <c r="E9" t="n">
-        <v>13000</v>
+        <v>13338</v>
       </c>
       <c r="F9" t="n">
-        <v>14985.03700215833</v>
+        <v>26157.21918486721</v>
       </c>
       <c r="G9" t="n">
-        <v>1985.037002158331</v>
+        <v>12819.21918486721</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45809.73307043832</v>
+        <v>45809.82485457524</v>
       </c>
       <c r="B10" t="n">
         <v>1000</v>
       </c>
       <c r="C10" t="n">
-        <v>5911.68994140625</v>
+        <v>65.31999969482422</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1691563681301804</v>
+        <v>15.30924685658315</v>
       </c>
       <c r="E10" t="n">
-        <v>14000</v>
+        <v>14338</v>
       </c>
       <c r="F10" t="n">
-        <v>16108.86119814316</v>
+        <v>27630.12181092304</v>
       </c>
       <c r="G10" t="n">
-        <v>2108.861198143162</v>
+        <v>13292.12181092304</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45839.73307043832</v>
+        <v>45839.82485457524</v>
       </c>
       <c r="B11" t="n">
-        <v>1000</v>
+        <v>1779</v>
       </c>
       <c r="C11" t="n">
-        <v>6198.009765625</v>
+        <v>67.58000183105469</v>
       </c>
       <c r="D11" t="n">
-        <v>0.1613421142938714</v>
+        <v>26.32435560518889</v>
       </c>
       <c r="E11" t="n">
-        <v>15000</v>
+        <v>16117</v>
       </c>
       <c r="F11" t="n">
-        <v>17180.76983438949</v>
+        <v>30162.7880395976</v>
       </c>
       <c r="G11" t="n">
-        <v>2180.769834389488</v>
+        <v>14045.7880395976</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45870.73307043832</v>
+        <v>45870.82485457524</v>
       </c>
       <c r="B12" t="n">
         <v>1000</v>
       </c>
       <c r="C12" t="n">
-        <v>6238.009765625</v>
+        <v>65.02999877929688</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1603075399962616</v>
+        <v>15.37751835724104</v>
       </c>
       <c r="E12" t="n">
-        <v>16000</v>
+        <v>17117</v>
       </c>
       <c r="F12" t="n">
-        <v>18245.80506917272</v>
+        <v>31642.25906666922</v>
       </c>
       <c r="G12" t="n">
-        <v>2245.805069172719</v>
+        <v>14525.25906666922</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45901.73307043832</v>
+        <v>45901.82485457524</v>
       </c>
       <c r="B13" t="n">
         <v>1000</v>
       </c>
       <c r="C13" t="n">
-        <v>6460.259765625</v>
+        <v>80.05000305175781</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1547925371857326</v>
+        <v>12.492191903521</v>
       </c>
       <c r="E13" t="n">
-        <v>17000</v>
+        <v>18117</v>
       </c>
       <c r="F13" t="n">
-        <v>19274.20027870648</v>
+        <v>32844.13283827003</v>
       </c>
       <c r="G13" t="n">
-        <v>2274.200278706485</v>
+        <v>14727.13283827003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>